<commit_message>
Trying to get g/l for category
</commit_message>
<xml_diff>
--- a/theme_track_config2.xlsx
+++ b/theme_track_config2.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="357">
   <si>
     <t xml:space="preserve">Options</t>
   </si>
@@ -54,7 +54,13 @@
     <t xml:space="preserve">3m;6m;1y</t>
   </si>
   <si>
-    <t xml:space="preserve">Performance as measured using yahoo finance periods wanted. ‘Xm’ = months, ‘Xy’ = years. For multiple, seperate with ‘;’. For each will create a new column ‘R:Performance&lt;Period&gt;’ which then can be referenced in the reports below</t>
+    <t xml:space="preserve">Performance as measured using yahoo finance periods wanted. ‘Xm’ = months, ‘Xy’ = years. For multiple, separate with ‘;’. For each will create a new column ‘R:Performance&lt;Period&gt;’ which then can be referenced in the reports below</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HistoricalPerformanceSlippageDays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the start date of the historical performance period falls on a weekend or holiday, or for some reason the data is missing, the date will be adjusted to the closest working day where there is data. This value is the maximum number of days an adjustment can be made before the data is considered invalid.</t>
   </si>
   <si>
     <t xml:space="preserve">ThemeReport</t>
@@ -1353,10 +1359,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ162"/>
+  <dimension ref="A1:AMJ163"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A71" activeCellId="0" sqref="71:73"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1414,16 +1420,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1442,104 +1451,104 @@
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="2" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="F10" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="3" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2" t="s">
+      <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="3"/>
+      <c r="F12" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="F13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="1" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3"/>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="8" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="C15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="D15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1547,7 +1556,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1557,57 +1566,54 @@
       <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="2" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3"/>
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="F23" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="A24" s="3"/>
+      <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="3" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="2" t="s">
+      <c r="B25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="6" t="s">
+      <c r="D25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="3"/>
+      <c r="F25" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1618,7 +1624,7 @@
         <v>40</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1629,54 +1635,52 @@
         <v>42</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="8"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3"/>
-      <c r="B32" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="6" t="s">
         <v>48</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E32" s="8"/>
     </row>
@@ -1689,7 +1693,7 @@
         <v>50</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E33" s="8"/>
     </row>
@@ -1702,36 +1706,41 @@
         <v>52</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3"/>
       <c r="B35" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" s="8"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="8"/>
+      <c r="D36" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="E36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="B37" s="1" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="8"/>
@@ -1739,7 +1748,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="8"/>
@@ -1747,50 +1756,50 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="B40" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="B41" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C42" s="6"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1798,7 +1807,7 @@
         <v>14</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1806,112 +1815,112 @@
         <v>16</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D48" s="3" t="s">
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E48" s="3"/>
-      <c r="F48" s="2" t="s">
+      <c r="B49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="3"/>
+      <c r="F49" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="F50" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D50" s="1" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3"/>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D51" s="8" t="s">
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3"/>
+      <c r="B52" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E51" s="8"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="s">
+      <c r="C52" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D52" s="8"/>
+      <c r="D52" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="E52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="B54" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3" t="s">
-        <v>35</v>
-      </c>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="3"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1919,7 +1928,7 @@
         <v>14</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1927,53 +1936,50 @@
         <v>16</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F63" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D63" s="3" t="s">
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="2" t="s">
+      <c r="B64" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E64" s="3"/>
+      <c r="F64" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F64" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="1" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1984,7 +1990,7 @@
         <v>40</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1995,54 +2001,52 @@
         <v>42</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D69" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E69" s="8"/>
+      <c r="D69" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D70" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E70" s="8"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E70" s="8"/>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3"/>
-      <c r="B71" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="6" t="s">
         <v>48</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E71" s="8"/>
     </row>
@@ -2055,7 +2059,7 @@
         <v>50</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E72" s="8"/>
     </row>
@@ -2068,7 +2072,7 @@
         <v>52</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E73" s="8"/>
     </row>
@@ -2077,144 +2081,146 @@
       <c r="B74" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C74" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E74" s="8"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="3"/>
+      <c r="B75" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C75" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D74" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E74" s="8"/>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="D75" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E75" s="8"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="B76" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="1" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="B79" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="B80" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="9"/>
-    </row>
-    <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="9"/>
+    </row>
+    <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="F84" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C84" s="3" t="s">
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C85" s="1" t="s">
+      <c r="B85" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="C85" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="F86" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="F87" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="F88" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="F89" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C90" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="F90" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>84</v>
@@ -2225,7 +2231,7 @@
         <v>85</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>86</v>
@@ -2236,18 +2242,18 @@
         <v>87</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F93" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>91</v>
@@ -2258,7 +2264,7 @@
         <v>92</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>93</v>
@@ -2269,18 +2275,18 @@
         <v>94</v>
       </c>
       <c r="C96" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F96" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>98</v>
@@ -2291,40 +2297,48 @@
         <v>99</v>
       </c>
       <c r="C98" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F98" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="F99" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F99" s="2" t="s">
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="3"/>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C100" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="3"/>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="3"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="5"/>
-      <c r="B105" s="5"/>
+      <c r="A105" s="3"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A106" s="5"/>
       <c r="B106" s="5"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2495,12 +2509,15 @@
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="5"/>
     </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B163" s="5"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F12" r:id="rId1" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
-    <hyperlink ref="F25" r:id="rId2" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
-    <hyperlink ref="F49" r:id="rId3" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
-    <hyperlink ref="F64" r:id="rId4" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
+    <hyperlink ref="F13" r:id="rId1" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
+    <hyperlink ref="F26" r:id="rId2" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
+    <hyperlink ref="F50" r:id="rId3" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
+    <hyperlink ref="F65" r:id="rId4" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2520,7 +2537,7 @@
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="1" sqref="71:73 A26"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2535,7 +2552,7 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AMJ1" s="5"/>
     </row>
@@ -2544,37 +2561,37 @@
     </row>
     <row r="3" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="AMJ4" s="5"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="AMJ5" s="5"/>
     </row>
     <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="AMJ6" s="5"/>
     </row>
@@ -2583,7 +2600,7 @@
     </row>
     <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="AMJ8" s="5"/>
     </row>
@@ -2592,10 +2609,10 @@
     </row>
     <row r="10" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>1</v>
@@ -2604,30 +2621,30 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D13" s="5" t="n">
         <v>2343</v>
@@ -2635,38 +2652,38 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D17" s="5" t="n">
         <v>1171</v>
@@ -2674,66 +2691,66 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2754,8 +2771,8 @@
   </sheetPr>
   <dimension ref="A1:AMI213"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="1" sqref="71:73 A22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2771,7 +2788,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4823,10 +4840,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -5852,10 +5869,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -6881,10 +6898,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -7910,10 +7927,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -9964,7 +9981,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -12016,11 +12033,11 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
@@ -13047,19 +13064,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -14084,10 +14101,10 @@
       <c r="A12" s="1"/>
       <c r="B12" s="3"/>
       <c r="C12" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="3"/>
@@ -16136,16 +16153,16 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -17169,113 +17186,113 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>152</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>6</v>
@@ -17283,30 +17300,30 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17315,261 +17332,261 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E60" s="1"/>
     </row>
@@ -17578,1270 +17595,1270 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="5" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="5" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E140" s="5" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="E142" s="5" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="E144" s="5" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="E146" s="5" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D148" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E148" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="E148" s="5" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="E150" s="5" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E152" s="5" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D154" s="5" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="E154" s="5" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="E156" s="5" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D158" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="E158" s="5" t="s">
         <v>287</v>
-      </c>
-      <c r="E158" s="5" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D160" s="5" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E160" s="5" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D162" s="5" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="E162" s="5" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D164" s="5" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E164" s="5" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D166" s="5" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="E166" s="5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E168" s="5" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D170" s="5" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="E170" s="5" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D172" s="5" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E172" s="5" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D174" s="5" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="E174" s="5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D176" s="5" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="E176" s="5" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D178" s="5" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E178" s="5" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D180" s="5" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="E180" s="5" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D182" s="5" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E182" s="5" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D184" s="5" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E184" s="5" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D186" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="E186" s="5" t="s">
         <v>325</v>
-      </c>
-      <c r="E186" s="5" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D188" s="5" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="E188" s="5" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D190" s="5" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E190" s="5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D192" s="5" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E192" s="5" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B194" s="5" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C194" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D194" s="5" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E194" s="5" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D196" s="5" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E196" s="5" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C198" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D198" s="5" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="E198" s="5" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C200" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D200" s="5" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="E200" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B202" s="5" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C202" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D202" s="5" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="E202" s="5" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C204" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D204" s="5" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E204" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C206" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D206" s="5" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E206" s="5" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B209" s="5" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C209" s="5" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D209" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E209" s="5" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B210" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B212" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C212" s="5" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D212" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E212" s="5" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B213" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now prints out historical performance periods, though still has some problems with display order of columns.
</commit_message>
<xml_diff>
--- a/theme_track_config2.xlsx
+++ b/theme_track_config2.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="354">
   <si>
     <t xml:space="preserve">Options</t>
   </si>
@@ -30,7 +30,7 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Config Version</t>
+    <t xml:space="preserve">ConfigVersion</t>
   </si>
   <si>
     <t xml:space="preserve">1.0</t>
@@ -51,7 +51,7 @@
     <t xml:space="preserve">HistoricalPerformancePeriods</t>
   </si>
   <si>
-    <t xml:space="preserve">3m;6m;1y</t>
+    <t xml:space="preserve">3m;6m;1y;2y;5y</t>
   </si>
   <si>
     <t xml:space="preserve">Performance as measured using yahoo finance periods wanted. ‘Xm’ = months, ‘Xy’ = years. For multiple, separate with ‘;’. For each will create a new column ‘R:Performance&lt;Period&gt;’ which then can be referenced in the reports below</t>
@@ -129,6 +129,15 @@
     <t xml:space="preserve">0.00%</t>
   </si>
   <si>
+    <t xml:space="preserve">R:GainLoss${HistoricalPerformancePeriods}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G/L % ${HistoricalPerformancePeriods}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:GainLossNotAllPresent${HistoricalPerformancePeriods}</t>
+  </si>
+  <si>
     <t xml:space="preserve">ColumnOrder</t>
   </si>
   <si>
@@ -171,24 +180,6 @@
     <t xml:space="preserve">% of Total</t>
   </si>
   <si>
-    <t xml:space="preserve">R:Performance3m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G/L % 3m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R:Performance6m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G/L % 6m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R:Performance1y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G/L % 1y</t>
-  </si>
-  <si>
     <t xml:space="preserve">R:Notes</t>
   </si>
   <si>
@@ -486,9 +477,18 @@
     <t xml:space="preserve">Currency</t>
   </si>
   <si>
+    <t xml:space="preserve">R:Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${qty}</t>
+  </si>
+  <si>
     <t xml:space="preserve">WhenGenerated</t>
   </si>
   <si>
+    <t xml:space="preserve">Quantity</t>
+  </si>
+  <si>
     <t xml:space="preserve">USA</t>
   </si>
   <si>
@@ -498,16 +498,7 @@
     <t xml:space="preserve">Mkt Val (Market Value)</t>
   </si>
   <si>
-    <t xml:space="preserve">\$?${value}</t>
-  </si>
-  <si>
     <t xml:space="preserve">Qty (Quantity)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${qty}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantity</t>
   </si>
   <si>
     <t xml:space="preserve">Pick</t>
@@ -1361,8 +1352,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ163"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1526,124 +1517,125 @@
       <c r="E15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3"/>
+      <c r="B17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="1" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="1" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="1" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3"/>
+      <c r="A24" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="B24" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3"/>
+      <c r="B26" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="2" t="s">
+      <c r="E27" s="3"/>
+      <c r="F27" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="F28" s="7" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>27</v>
@@ -1651,13 +1643,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1667,29 +1659,26 @@
       <c r="C31" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D31" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="8"/>
+      <c r="D32" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3"/>
       <c r="B33" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D33" s="8" t="s">
@@ -1697,13 +1686,12 @@
       </c>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3"/>
+    <row r="34" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>34</v>
@@ -1713,10 +1701,10 @@
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
       <c r="B35" s="1" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>34</v>
@@ -1725,7 +1713,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>1</v>
@@ -1737,7 +1725,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>17</v>
@@ -1748,7 +1736,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="8"/>
@@ -1756,7 +1744,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="8"/>
@@ -1764,7 +1752,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="8"/>
@@ -1772,7 +1760,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>29</v>
@@ -1807,7 +1795,7 @@
         <v>14</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1815,7 +1803,7 @@
         <v>16</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1823,7 +1811,7 @@
         <v>18</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>20</v>
@@ -1849,10 +1837,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>27</v>
@@ -1886,130 +1874,131 @@
       <c r="E52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="3"/>
+      <c r="B53" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D53" s="8"/>
+      <c r="C53" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="E53" s="8"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="A54" s="3"/>
       <c r="B54" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" s="8"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="1" t="s">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="3"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="3"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="3"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="A60" s="3"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D66" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E64" s="3"/>
-      <c r="F64" s="2" t="s">
+      <c r="E66" s="3"/>
+      <c r="F66" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F65" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="1" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="F67" s="7" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C68" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>27</v>
@@ -2017,13 +2006,13 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="1" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2033,29 +2022,26 @@
       <c r="C70" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D70" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E70" s="8"/>
+      <c r="D70" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D71" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E71" s="8"/>
+      <c r="D71" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="3"/>
       <c r="B72" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D72" s="8" t="s">
@@ -2064,12 +2050,11 @@
       <c r="E72" s="8"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="3"/>
       <c r="B73" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C73" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>34</v>
@@ -2079,10 +2064,10 @@
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3"/>
       <c r="B74" s="1" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>34</v>
@@ -2092,7 +2077,7 @@
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3"/>
       <c r="B75" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>1</v>
@@ -2104,30 +2089,30 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>29</v>
@@ -2143,21 +2128,21 @@
     </row>
     <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2165,164 +2150,164 @@
         <v>6</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2515,9 +2500,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F13" r:id="rId1" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
-    <hyperlink ref="F26" r:id="rId2" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
+    <hyperlink ref="F28" r:id="rId2" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
     <hyperlink ref="F50" r:id="rId3" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
-    <hyperlink ref="F65" r:id="rId4" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
+    <hyperlink ref="F67" r:id="rId4" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2552,7 +2537,7 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="AMJ1" s="5"/>
     </row>
@@ -2561,37 +2546,37 @@
     </row>
     <row r="3" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AMJ4" s="5"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AMJ5" s="5"/>
     </row>
     <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="AMJ6" s="5"/>
     </row>
@@ -2600,7 +2585,7 @@
     </row>
     <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AMJ8" s="5"/>
     </row>
@@ -2609,10 +2594,10 @@
     </row>
     <row r="10" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>1</v>
@@ -2621,30 +2606,30 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D13" s="5" t="n">
         <v>2343</v>
@@ -2652,38 +2637,38 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D17" s="5" t="n">
         <v>1171</v>
@@ -2691,66 +2676,66 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2771,7 +2756,7 @@
   </sheetPr>
   <dimension ref="A1:AMI213"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A178" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -2788,7 +2773,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4840,10 +4825,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -5869,10 +5854,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -6898,10 +6883,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -7927,10 +7912,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -9981,7 +9966,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -12033,11 +12018,11 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
@@ -13064,19 +13049,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -14101,10 +14086,10 @@
       <c r="A12" s="1"/>
       <c r="B12" s="3"/>
       <c r="C12" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="3"/>
@@ -16153,16 +16138,16 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -17186,85 +17171,99 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>148</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>155</v>
@@ -17272,27 +17271,27 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>156</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>6</v>
@@ -17303,27 +17302,27 @@
         <v>157</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17332,90 +17331,90 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>165</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17423,29 +17422,29 @@
         <v>26</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17453,140 +17452,140 @@
         <v>26</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E60" s="1"/>
     </row>
@@ -17595,13 +17594,13 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>155</v>
@@ -17609,71 +17608,71 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>156</v>
@@ -17681,1184 +17680,1184 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C74" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C74" s="5" t="s">
-        <v>190</v>
-      </c>
       <c r="D74" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B92" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E92" s="5" t="s">
         <v>200</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E140" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E142" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E144" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E146" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E148" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E150" s="5" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E152" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D154" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E154" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E156" s="5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D158" s="5" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E158" s="5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D160" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E160" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D162" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E162" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D164" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E164" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D166" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E166" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E168" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D170" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E170" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D172" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E172" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D174" s="5" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E174" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D176" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E176" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D178" s="5" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E178" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D180" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E180" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D182" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E182" s="5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D184" s="5" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E184" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D186" s="5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E186" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D188" s="5" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E188" s="5" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D190" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E190" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D192" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E192" s="5" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B194" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C194" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D194" s="5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E194" s="5" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D196" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E196" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C198" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D198" s="5" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E198" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C200" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D200" s="5" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E200" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B202" s="5" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C202" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D202" s="5" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E202" s="5" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C204" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D204" s="5" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E204" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C206" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D206" s="5" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E206" s="5" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B209" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="C209" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="D209" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="E209" s="5" t="s">
         <v>352</v>
-      </c>
-      <c r="C209" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="D209" s="5" t="s">
-        <v>354</v>
-      </c>
-      <c r="E209" s="5" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B210" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B212" s="5" t="s">
         <v>155</v>
       </c>
       <c r="C212" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="D212" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E212" s="5" t="s">
         <v>353</v>
-      </c>
-      <c r="D212" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="E212" s="5" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B213" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>